<commit_message>
fixed excel blank template
</commit_message>
<xml_diff>
--- a/prev_sheets/blank_example.xlsx
+++ b/prev_sheets/blank_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dopal\Box Sync\lab_graphic_dist_clean\prev_graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dopal\Desktop\lab_graphic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95BD675-0916-4565-8B28-3B8F1E2D9E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB539D4-4A54-4025-B28A-4184604F33D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="-405" windowWidth="21600" windowHeight="11385" tabRatio="538" activeTab="1" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="538" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Mice" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>DATE</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>STUDY LEGEND</t>
-  </si>
-  <si>
     <t>Status/Condition</t>
   </si>
   <si>
@@ -88,15 +85,42 @@
   </si>
   <si>
     <t>Wean Date</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>B234</t>
+  </si>
+  <si>
+    <t>Breeding</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,9 +158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,16 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D288F3BE-204A-46EE-B197-DA56EF367A3F}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="37.5703125" customWidth="1"/>
@@ -477,7 +504,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
@@ -498,7 +525,7 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -521,6 +548,38 @@
       </c>
       <c r="L2" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4">
+        <v>36526</v>
+      </c>
+      <c r="F3">
+        <v>562</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -530,51 +589,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A29D230-8104-4AD8-AFDD-EF632F2A3945}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
-      <c r="G1" t="s">
-        <v>13</v>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>36526</v>
+      </c>
+      <c r="E3" s="4">
+        <v>36526</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished new feature for death/sack date print
</commit_message>
<xml_diff>
--- a/prev_sheets/blank_example.xlsx
+++ b/prev_sheets/blank_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dopal\Desktop\lab_graphic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dopal\Desktop\lab_graphic_project\prev_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB539D4-4A54-4025-B28A-4184604F33D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5ACDEF-5122-4984-B865-F06E2B47A4F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="538" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" tabRatio="538" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Mice" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>Pregnant?</t>
   </si>
   <si>
-    <t>Sacked Status: Potential (P), Sacked (S)</t>
-  </si>
-  <si>
-    <t>Date of Sack</t>
-  </si>
-  <si>
     <t>Genotyped?</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Date of Death</t>
+  </si>
+  <si>
+    <t>Sacked Status: Potential (P), Sacked (S), Sacrificed(D)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,8 +490,8 @@
     <col min="5" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
@@ -507,7 +507,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="1"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -535,19 +535,19 @@
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -555,13 +555,13 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4">
         <v>36526</v>
@@ -570,20 +570,21 @@
         <v>562</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -613,7 +614,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -621,30 +622,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -656,10 +657,10 @@
         <v>36526</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new prev_sheets; strip whitespace; reformat logs
</commit_message>
<xml_diff>
--- a/prev_sheets/blank_example.xlsx
+++ b/prev_sheets/blank_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dopal\Desktop\lab_graphic_project\prev_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5ACDEF-5122-4984-B865-F06E2B47A4F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4149C24-3743-4387-83DE-88593D94A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11385" tabRatio="538" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
+    <workbookView xWindow="3345" yWindow="3270" windowWidth="21600" windowHeight="11385" tabRatio="538" xr2:uid="{8BC872A1-ADDA-4203-97AB-B18266E290E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Mice" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
     <t>Date of Death</t>
   </si>
   <si>
-    <t>Sacked Status: Potential (P), Sacked (S), Sacrificed(D)</t>
+    <t>Sacked Status: Potential (P), Sacked (S), Died (D)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>